<commit_message>
I did more dynamic and added READ.md page
</commit_message>
<xml_diff>
--- a/src/test/resources/Customers.xlsx
+++ b/src/test/resources/Customers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alitokmak/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alitokmak/IdeaProjects/_4CInsights/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E5DE919-47AC-4B42-8FE6-09F05CE78E7F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D360B8DE-B9D4-BC45-BBD4-A4853B2902C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16120" xr2:uid="{C69F1D51-1562-6642-AC89-CFC53F87EC86}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>user5</t>
+  </si>
+  <si>
+    <t>abc</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B3" sqref="B3:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -423,40 +426,40 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>123</v>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
-      <c r="B4">
-        <v>123</v>
+      <c r="B4" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
-        <v>123</v>
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>123</v>
+      <c r="B6" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>